<commit_message>
corrección de 2 fechas
</commit_message>
<xml_diff>
--- a/Estimación/Gantt FashionProject .xlsx
+++ b/Estimación/Gantt FashionProject .xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexndr/Desktop/TallerIngSoft/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="22720" windowHeight="14600" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="FashionProject" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Comments" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="FashionProject" sheetId="1" r:id="rId1"/>
+    <sheet name="Comments" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -23,466 +30,464 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="150">
   <si>
-    <t xml:space="preserve">Estado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre de la tarea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha de Inicio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asignado a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">% Completado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duración</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Predecesores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comentarios</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nivelación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reunión para nivelar información sobre el proyecto.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremento 1 - Gestión de Clientes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresar cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Análisis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,5d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Análisis de requerimientos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diseño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diseñar interfaz usando prototipos.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Implementación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desarrollar código del sistema.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Realizar pruebas de testeo del ejecutable.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Documentación</t>
-  </si>
-  <si>
-    <t xml:space="preserve">María José</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camilo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cambiar estado cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Humberto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremento 2 - Administrar Trabajadores</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresar trabajador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gabriel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar trabajador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cambiar estado trabajador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremento 3 - Gestión de Tratamientos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresar tratamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar tratamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cambiar estado tratamiento</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremento 4 - Registrar Ventas</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrar un servicio dado (venta) a un cliente registrado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Registrar un servicio dado (venta) a un cliente sin registrar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremento 5 - Administrar Gastos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingresar gastos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Editar monto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eliminar gasto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87</t>
-  </si>
-  <si>
-    <t xml:space="preserve">88</t>
-  </si>
-  <si>
-    <t xml:space="preserve">89</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremento 6 - Informes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar informe de gastos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90</t>
-  </si>
-  <si>
-    <t xml:space="preserve">93</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94</t>
-  </si>
-  <si>
-    <t xml:space="preserve">95</t>
-  </si>
-  <si>
-    <t xml:space="preserve">96</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar informe de ganancias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">97</t>
-  </si>
-  <si>
-    <t xml:space="preserve">99</t>
-  </si>
-  <si>
-    <t xml:space="preserve">100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">102</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Generar informe de trabajador</t>
-  </si>
-  <si>
-    <t xml:space="preserve">103</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">106</t>
-  </si>
-  <si>
-    <t xml:space="preserve">107</t>
-  </si>
-  <si>
-    <t xml:space="preserve">108</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incremento 7 – Lo-gin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Autenticarse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">112</t>
-  </si>
-  <si>
-    <t xml:space="preserve">113</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114</t>
-  </si>
-  <si>
-    <t xml:space="preserve">115</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificación Final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pruebas del sistema final</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pruebas para días Martes y Miércoles.</t>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>Nombre de la tarea</t>
+  </si>
+  <si>
+    <t>Fecha de Inicio</t>
+  </si>
+  <si>
+    <t>Fecha final</t>
+  </si>
+  <si>
+    <t>Asignado a</t>
+  </si>
+  <si>
+    <t>% Completado</t>
+  </si>
+  <si>
+    <t>Duración</t>
+  </si>
+  <si>
+    <t>Predecesores</t>
+  </si>
+  <si>
+    <t>Comentarios</t>
+  </si>
+  <si>
+    <t>Nivelación</t>
+  </si>
+  <si>
+    <t>2d</t>
+  </si>
+  <si>
+    <t>Reunión para nivelar información sobre el proyecto.</t>
+  </si>
+  <si>
+    <t>Incremento 1 - Gestión de Clientes</t>
+  </si>
+  <si>
+    <t>12d</t>
+  </si>
+  <si>
+    <t>Ingresar cliente</t>
+  </si>
+  <si>
+    <t>4d</t>
+  </si>
+  <si>
+    <t>Análisis</t>
+  </si>
+  <si>
+    <t>0,5d</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Análisis de requerimientos.</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Diseñar interfaz usando prototipos.</t>
+  </si>
+  <si>
+    <t>Implementación</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Desarrollar código del sistema.</t>
+  </si>
+  <si>
+    <t>Verificación</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Realizar pruebas de testeo del ejecutable.</t>
+  </si>
+  <si>
+    <t>Documentación</t>
+  </si>
+  <si>
+    <t>María José</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Editar cliente</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Camilo</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Cambiar estado cliente</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Humberto</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>Incremento 2 - Administrar Trabajadores</t>
+  </si>
+  <si>
+    <t>Ingresar trabajador</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>Editar trabajador</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>Cambiar estado trabajador</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>36</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>Incremento 3 - Gestión de Tratamientos</t>
+  </si>
+  <si>
+    <t>Ingresar tratamiento</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>Editar tratamiento</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Cambiar estado tratamiento</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>Incremento 4 - Registrar Ventas</t>
+  </si>
+  <si>
+    <t>8d</t>
+  </si>
+  <si>
+    <t>Registrar un servicio dado (venta) a un cliente registrado</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>Registrar un servicio dado (venta) a un cliente sin registrar</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t>69</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>Incremento 5 - Administrar Gastos</t>
+  </si>
+  <si>
+    <t>9d</t>
+  </si>
+  <si>
+    <t>Ingresar gastos</t>
+  </si>
+  <si>
+    <t>3d</t>
+  </si>
+  <si>
+    <t>71</t>
+  </si>
+  <si>
+    <t>74</t>
+  </si>
+  <si>
+    <t>1d</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>77</t>
+  </si>
+  <si>
+    <t>Editar monto</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>Eliminar gasto</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>Incremento 6 - Informes</t>
+  </si>
+  <si>
+    <t>Generar informe de gastos</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>Generar informe de ganancias</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>Generar informe de trabajador</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>Incremento 7 – Lo-gin</t>
+  </si>
+  <si>
+    <t>Autenticarse</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>Verificación Final</t>
+  </si>
+  <si>
+    <t>Pruebas del sistema final</t>
+  </si>
+  <si>
+    <t>Pruebas para días Martes y Miércoles.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="#,##0%;\-#,##0%"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0%;\-#,##0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -491,34 +496,17 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -532,7 +520,6 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -557,7 +544,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -565,113 +552,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="4" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="4"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -730,37 +668,296 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I119"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B121" activeCellId="0" sqref="B121"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="H86" sqref="H86"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.7773279352227"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1052631578947"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.74898785425101"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.35627530364373"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="39.6356275303644"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.89068825910931"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -789,19 +986,19 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="26" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="n">
+      <c r="C2" s="4">
         <v>42958</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="4">
         <v>42960</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="5" t="n">
+      <c r="F2" s="5">
         <v>0</v>
       </c>
       <c r="G2" s="2" t="s">
@@ -812,19 +1009,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="65" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="4">
         <v>42961</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="4">
         <v>42981</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="5">
         <v>0</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -833,19 +1030,19 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="4" spans="1:9" ht="39" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="9">
         <v>42961</v>
       </c>
-      <c r="D4" s="9" t="n">
+      <c r="D4" s="9">
         <v>42967</v>
       </c>
       <c r="E4" s="10"/>
-      <c r="F4" s="11" t="n">
+      <c r="F4" s="11">
         <v>0</v>
       </c>
       <c r="G4" s="10" t="s">
@@ -854,19 +1051,19 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="5" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="13" t="n">
+      <c r="C5" s="13">
         <v>42961</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="13">
         <v>42961</v>
       </c>
       <c r="E5" s="7"/>
-      <c r="F5" s="14" t="n">
+      <c r="F5" s="14">
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
@@ -879,19 +1076,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="6" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="13" t="n">
+      <c r="C6" s="13">
         <v>42961</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="13">
         <v>42961</v>
       </c>
       <c r="E6" s="7"/>
-      <c r="F6" s="14" t="n">
+      <c r="F6" s="14">
         <v>0</v>
       </c>
       <c r="G6" s="7" t="s">
@@ -904,19 +1101,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="7" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="13" t="n">
+      <c r="C7" s="13">
         <v>42963</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="13">
         <v>42965</v>
       </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="14" t="n">
+      <c r="F7" s="14">
         <v>0</v>
       </c>
       <c r="G7" s="7" t="s">
@@ -929,19 +1126,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="8" spans="1:9" ht="39" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
       <c r="B8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="13" t="n">
+      <c r="C8" s="13">
         <v>42967</v>
       </c>
-      <c r="D8" s="13" t="n">
+      <c r="D8" s="13">
         <v>42967</v>
       </c>
       <c r="E8" s="7"/>
-      <c r="F8" s="14" t="n">
+      <c r="F8" s="14">
         <v>0</v>
       </c>
       <c r="G8" s="7" t="s">
@@ -954,21 +1151,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="9" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
       <c r="B9" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="13" t="n">
+      <c r="C9" s="13">
         <v>42967</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="13">
         <v>42967</v>
       </c>
       <c r="E9" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="14" t="n">
+      <c r="F9" s="14">
         <v>0</v>
       </c>
       <c r="G9" s="7" t="s">
@@ -979,19 +1176,19 @@
       </c>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="10" spans="1:9" ht="26" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7"/>
       <c r="B10" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="9">
         <v>42968</v>
       </c>
-      <c r="D10" s="9" t="n">
-        <v>43005</v>
+      <c r="D10" s="9">
+        <v>42974</v>
       </c>
       <c r="E10" s="10"/>
-      <c r="F10" s="11" t="n">
+      <c r="F10" s="11">
         <v>0</v>
       </c>
       <c r="G10" s="10" t="s">
@@ -1000,19 +1197,19 @@
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="11" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A11" s="7"/>
       <c r="B11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="13" t="n">
+      <c r="C11" s="13">
         <v>42968</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="13">
         <v>42968</v>
       </c>
       <c r="E11" s="7"/>
-      <c r="F11" s="14" t="n">
+      <c r="F11" s="14">
         <v>0</v>
       </c>
       <c r="G11" s="7" t="s">
@@ -1025,19 +1222,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="12" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="13" t="n">
+      <c r="C12" s="13">
         <v>42968</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="13">
         <v>42968</v>
       </c>
       <c r="E12" s="7"/>
-      <c r="F12" s="14" t="n">
+      <c r="F12" s="14">
         <v>0</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -1050,19 +1247,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="13" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
       <c r="B13" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="13" t="n">
+      <c r="C13" s="13">
         <v>42970</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="13">
         <v>42972</v>
       </c>
       <c r="E13" s="7"/>
-      <c r="F13" s="14" t="n">
+      <c r="F13" s="14">
         <v>0</v>
       </c>
       <c r="G13" s="7" t="s">
@@ -1075,19 +1272,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="14" spans="1:9" ht="39" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="13" t="n">
+      <c r="C14" s="13">
         <v>42974</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="13">
         <v>42974</v>
       </c>
       <c r="E14" s="7"/>
-      <c r="F14" s="14" t="n">
+      <c r="F14" s="14">
         <v>0</v>
       </c>
       <c r="G14" s="7" t="s">
@@ -1100,21 +1297,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="15" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
       <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="13" t="n">
+      <c r="C15" s="13">
         <v>42974</v>
       </c>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="13">
         <v>42974</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="14" t="n">
+      <c r="F15" s="14">
         <v>0</v>
       </c>
       <c r="G15" s="7" t="s">
@@ -1125,19 +1322,19 @@
       </c>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="16" spans="1:9" ht="65" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
       <c r="B16" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="9">
         <v>42975</v>
       </c>
-      <c r="D16" s="9" t="n">
+      <c r="D16" s="9">
         <v>42981</v>
       </c>
       <c r="E16" s="10"/>
-      <c r="F16" s="11" t="n">
+      <c r="F16" s="11">
         <v>0</v>
       </c>
       <c r="G16" s="10" t="s">
@@ -1146,19 +1343,19 @@
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="17" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="13" t="n">
+      <c r="C17" s="13">
         <v>42975</v>
       </c>
-      <c r="D17" s="13" t="n">
+      <c r="D17" s="13">
         <v>42975</v>
       </c>
       <c r="E17" s="7"/>
-      <c r="F17" s="14" t="n">
+      <c r="F17" s="14">
         <v>0</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -1171,19 +1368,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="18" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A18" s="7"/>
       <c r="B18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="13" t="n">
+      <c r="C18" s="13">
         <v>42975</v>
       </c>
-      <c r="D18" s="13" t="n">
+      <c r="D18" s="13">
         <v>42975</v>
       </c>
       <c r="E18" s="7"/>
-      <c r="F18" s="14" t="n">
+      <c r="F18" s="14">
         <v>0</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -1196,19 +1393,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="19" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A19" s="7"/>
       <c r="B19" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="13" t="n">
+      <c r="C19" s="13">
         <v>42977</v>
       </c>
-      <c r="D19" s="13" t="n">
+      <c r="D19" s="13">
         <v>42979</v>
       </c>
       <c r="E19" s="7"/>
-      <c r="F19" s="14" t="n">
+      <c r="F19" s="14">
         <v>0</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -1221,19 +1418,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="20" spans="1:9" ht="39" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="13" t="n">
+      <c r="C20" s="13">
         <v>42981</v>
       </c>
-      <c r="D20" s="13" t="n">
+      <c r="D20" s="13">
         <v>42981</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="14" t="n">
+      <c r="F20" s="14">
         <v>0</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -1246,21 +1443,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="21" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A21" s="7"/>
       <c r="B21" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="13" t="n">
+      <c r="C21" s="13">
         <v>42981</v>
       </c>
-      <c r="D21" s="13" t="n">
+      <c r="D21" s="13">
         <v>42981</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="14" t="n">
+      <c r="F21" s="14">
         <v>0</v>
       </c>
       <c r="G21" s="7" t="s">
@@ -1271,19 +1468,19 @@
       </c>
       <c r="I21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:9" ht="78" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="4" t="n">
+      <c r="C22" s="4">
         <v>42982</v>
       </c>
-      <c r="D22" s="4" t="n">
+      <c r="D22" s="4">
         <v>43002</v>
       </c>
       <c r="E22" s="2"/>
-      <c r="F22" s="5" t="n">
+      <c r="F22" s="5">
         <v>0</v>
       </c>
       <c r="G22" s="2" t="s">
@@ -1292,19 +1489,19 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="23" spans="1:9" ht="52" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7"/>
       <c r="B23" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="9">
         <v>42982</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="9">
         <v>42988</v>
       </c>
       <c r="E23" s="10"/>
-      <c r="F23" s="11" t="n">
+      <c r="F23" s="11">
         <v>0</v>
       </c>
       <c r="G23" s="10" t="s">
@@ -1313,19 +1510,19 @@
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="24" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A24" s="7"/>
       <c r="B24" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="13" t="n">
+      <c r="C24" s="13">
         <v>42982</v>
       </c>
-      <c r="D24" s="13" t="n">
+      <c r="D24" s="13">
         <v>42982</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="14" t="n">
+      <c r="F24" s="14">
         <v>0</v>
       </c>
       <c r="G24" s="7" t="s">
@@ -1338,19 +1535,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="25" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A25" s="7"/>
       <c r="B25" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="13" t="n">
+      <c r="C25" s="13">
         <v>42982</v>
       </c>
-      <c r="D25" s="13" t="n">
+      <c r="D25" s="13">
         <v>42982</v>
       </c>
       <c r="E25" s="7"/>
-      <c r="F25" s="14" t="n">
+      <c r="F25" s="14">
         <v>0</v>
       </c>
       <c r="G25" s="7" t="s">
@@ -1363,19 +1560,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="26" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A26" s="7"/>
       <c r="B26" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="13" t="n">
+      <c r="C26" s="13">
         <v>42984</v>
       </c>
-      <c r="D26" s="13" t="n">
+      <c r="D26" s="13">
         <v>43016</v>
       </c>
       <c r="E26" s="7"/>
-      <c r="F26" s="14" t="n">
+      <c r="F26" s="14">
         <v>0</v>
       </c>
       <c r="G26" s="7" t="s">
@@ -1388,19 +1585,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="27" spans="1:9" ht="39" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A27" s="7"/>
       <c r="B27" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="13" t="n">
+      <c r="C27" s="13">
         <v>43018</v>
       </c>
-      <c r="D27" s="13" t="n">
+      <c r="D27" s="13">
         <v>43018</v>
       </c>
       <c r="E27" s="7"/>
-      <c r="F27" s="14" t="n">
+      <c r="F27" s="14">
         <v>0</v>
       </c>
       <c r="G27" s="7" t="s">
@@ -1413,21 +1610,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="28" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A28" s="7"/>
       <c r="B28" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C28" s="13" t="n">
+      <c r="C28" s="13">
         <v>43018</v>
       </c>
-      <c r="D28" s="13" t="n">
+      <c r="D28" s="13">
         <v>43018</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F28" s="14" t="n">
+      <c r="F28" s="14">
         <v>0</v>
       </c>
       <c r="G28" s="7" t="s">
@@ -1438,19 +1635,19 @@
       </c>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="29" spans="1:9" ht="39" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7"/>
       <c r="B29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="9">
         <v>42989</v>
       </c>
-      <c r="D29" s="9" t="n">
+      <c r="D29" s="9">
         <v>42995</v>
       </c>
       <c r="E29" s="10"/>
-      <c r="F29" s="11" t="n">
+      <c r="F29" s="11">
         <v>0</v>
       </c>
       <c r="G29" s="10" t="s">
@@ -1459,19 +1656,19 @@
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
     </row>
-    <row r="30" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="30" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A30" s="7"/>
       <c r="B30" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="13" t="n">
+      <c r="C30" s="13">
         <v>42989</v>
       </c>
-      <c r="D30" s="13" t="n">
+      <c r="D30" s="13">
         <v>42989</v>
       </c>
       <c r="E30" s="7"/>
-      <c r="F30" s="14" t="n">
+      <c r="F30" s="14">
         <v>0</v>
       </c>
       <c r="G30" s="7" t="s">
@@ -1484,19 +1681,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="31" spans="1:9" ht="26" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A31" s="7"/>
       <c r="B31" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="13" t="n">
+      <c r="C31" s="13">
         <v>42989</v>
       </c>
-      <c r="D31" s="13" t="n">
+      <c r="D31" s="13">
         <v>42989</v>
       </c>
       <c r="E31" s="7"/>
-      <c r="F31" s="14" t="n">
+      <c r="F31" s="14">
         <v>0</v>
       </c>
       <c r="G31" s="7" t="s">
@@ -1509,19 +1706,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="32" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A32" s="7"/>
       <c r="B32" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="13" t="n">
+      <c r="C32" s="13">
         <v>42991</v>
       </c>
-      <c r="D32" s="13" t="n">
+      <c r="D32" s="13">
         <v>42993</v>
       </c>
       <c r="E32" s="7"/>
-      <c r="F32" s="14" t="n">
+      <c r="F32" s="14">
         <v>0</v>
       </c>
       <c r="G32" s="7" t="s">
@@ -1534,19 +1731,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="33" spans="1:9" ht="39" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A33" s="7"/>
       <c r="B33" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C33" s="13" t="n">
+      <c r="C33" s="13">
         <v>42995</v>
       </c>
-      <c r="D33" s="13" t="n">
+      <c r="D33" s="13">
         <v>42995</v>
       </c>
       <c r="E33" s="7"/>
-      <c r="F33" s="14" t="n">
+      <c r="F33" s="14">
         <v>0</v>
       </c>
       <c r="G33" s="7" t="s">
@@ -1559,21 +1756,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="34" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A34" s="7"/>
       <c r="B34" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C34" s="13" t="n">
+      <c r="C34" s="13">
         <v>42995</v>
       </c>
-      <c r="D34" s="13" t="n">
+      <c r="D34" s="13">
         <v>42995</v>
       </c>
       <c r="E34" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F34" s="14" t="n">
+      <c r="F34" s="14">
         <v>0</v>
       </c>
       <c r="G34" s="7" t="s">
@@ -1584,19 +1781,19 @@
       </c>
       <c r="I34" s="7"/>
     </row>
-    <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="35" spans="1:9" ht="78" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7"/>
       <c r="B35" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C35" s="9" t="n">
+      <c r="C35" s="9">
         <v>42996</v>
       </c>
-      <c r="D35" s="9" t="n">
+      <c r="D35" s="9">
         <v>43002</v>
       </c>
       <c r="E35" s="10"/>
-      <c r="F35" s="11" t="n">
+      <c r="F35" s="11">
         <v>0</v>
       </c>
       <c r="G35" s="10" t="s">
@@ -1605,19 +1802,19 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="36" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A36" s="7"/>
       <c r="B36" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C36" s="13" t="n">
+      <c r="C36" s="13">
         <v>43026</v>
       </c>
-      <c r="D36" s="13" t="n">
+      <c r="D36" s="13">
         <v>43026</v>
       </c>
       <c r="E36" s="7"/>
-      <c r="F36" s="14" t="n">
+      <c r="F36" s="14">
         <v>0</v>
       </c>
       <c r="G36" s="7" t="s">
@@ -1630,19 +1827,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="37" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A37" s="7"/>
       <c r="B37" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="13" t="n">
+      <c r="C37" s="13">
         <v>43026</v>
       </c>
-      <c r="D37" s="13" t="n">
+      <c r="D37" s="13">
         <v>43026</v>
       </c>
       <c r="E37" s="7"/>
-      <c r="F37" s="14" t="n">
+      <c r="F37" s="14">
         <v>0</v>
       </c>
       <c r="G37" s="7" t="s">
@@ -1655,19 +1852,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="38" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A38" s="7"/>
       <c r="B38" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="13" t="n">
+      <c r="C38" s="13">
         <v>43028</v>
       </c>
-      <c r="D38" s="13" t="n">
+      <c r="D38" s="13">
         <v>43030</v>
       </c>
       <c r="E38" s="7"/>
-      <c r="F38" s="14" t="n">
+      <c r="F38" s="14">
         <v>0</v>
       </c>
       <c r="G38" s="7" t="s">
@@ -1680,19 +1877,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="39" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39" s="7"/>
       <c r="B39" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="13" t="n">
+      <c r="C39" s="13">
         <v>43032</v>
       </c>
-      <c r="D39" s="13" t="n">
+      <c r="D39" s="13">
         <v>43032</v>
       </c>
       <c r="E39" s="7"/>
-      <c r="F39" s="14" t="n">
+      <c r="F39" s="14">
         <v>0</v>
       </c>
       <c r="G39" s="7" t="s">
@@ -1705,21 +1902,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="40" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A40" s="7"/>
       <c r="B40" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="13" t="n">
+      <c r="C40" s="13">
         <v>43032</v>
       </c>
-      <c r="D40" s="13" t="n">
+      <c r="D40" s="13">
         <v>43032</v>
       </c>
       <c r="E40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F40" s="14" t="n">
+      <c r="F40" s="14">
         <v>0</v>
       </c>
       <c r="G40" s="7" t="s">
@@ -1730,19 +1927,19 @@
       </c>
       <c r="I40" s="7"/>
     </row>
-    <row r="41" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:9" ht="78" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
       <c r="B41" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C41" s="4" t="n">
+      <c r="C41" s="4">
         <v>43003</v>
       </c>
-      <c r="D41" s="4" t="n">
+      <c r="D41" s="4">
         <v>43023</v>
       </c>
       <c r="E41" s="2"/>
-      <c r="F41" s="5" t="n">
+      <c r="F41" s="5">
         <v>0</v>
       </c>
       <c r="G41" s="2" t="s">
@@ -1751,19 +1948,19 @@
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="42" spans="1:9" ht="52" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7"/>
       <c r="B42" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C42" s="9" t="n">
+      <c r="C42" s="9">
         <v>43003</v>
       </c>
-      <c r="D42" s="9" t="n">
+      <c r="D42" s="9">
         <v>43009</v>
       </c>
       <c r="E42" s="10"/>
-      <c r="F42" s="11" t="n">
+      <c r="F42" s="11">
         <v>0</v>
       </c>
       <c r="G42" s="10" t="s">
@@ -1772,19 +1969,19 @@
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="43" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A43" s="7"/>
       <c r="B43" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="13" t="n">
+      <c r="C43" s="13">
         <v>43003</v>
       </c>
-      <c r="D43" s="13" t="n">
+      <c r="D43" s="13">
         <v>43003</v>
       </c>
       <c r="E43" s="7"/>
-      <c r="F43" s="14" t="n">
+      <c r="F43" s="14">
         <v>0</v>
       </c>
       <c r="G43" s="7" t="s">
@@ -1797,19 +1994,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="44" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A44" s="7"/>
       <c r="B44" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="13" t="n">
+      <c r="C44" s="13">
         <v>43003</v>
       </c>
-      <c r="D44" s="13" t="n">
+      <c r="D44" s="13">
         <v>43003</v>
       </c>
       <c r="E44" s="7"/>
-      <c r="F44" s="14" t="n">
+      <c r="F44" s="14">
         <v>0</v>
       </c>
       <c r="G44" s="7" t="s">
@@ -1822,19 +2019,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="45" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A45" s="7"/>
       <c r="B45" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C45" s="13" t="n">
+      <c r="C45" s="13">
         <v>43005</v>
       </c>
-      <c r="D45" s="13" t="n">
+      <c r="D45" s="13">
         <v>43007</v>
       </c>
       <c r="E45" s="7"/>
-      <c r="F45" s="14" t="n">
+      <c r="F45" s="14">
         <v>0</v>
       </c>
       <c r="G45" s="7" t="s">
@@ -1847,19 +2044,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="46" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A46" s="7"/>
       <c r="B46" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C46" s="13" t="n">
+      <c r="C46" s="13">
         <v>43009</v>
       </c>
-      <c r="D46" s="13" t="n">
+      <c r="D46" s="13">
         <v>43009</v>
       </c>
       <c r="E46" s="7"/>
-      <c r="F46" s="14" t="n">
+      <c r="F46" s="14">
         <v>0</v>
       </c>
       <c r="G46" s="7" t="s">
@@ -1872,21 +2069,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="47" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A47" s="7"/>
       <c r="B47" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="13" t="n">
+      <c r="C47" s="13">
         <v>43009</v>
       </c>
-      <c r="D47" s="13" t="n">
+      <c r="D47" s="13">
         <v>43009</v>
       </c>
       <c r="E47" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F47" s="14" t="n">
+      <c r="F47" s="14">
         <v>0</v>
       </c>
       <c r="G47" s="7" t="s">
@@ -1897,19 +2094,19 @@
       </c>
       <c r="I47" s="7"/>
     </row>
-    <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="48" spans="1:9" ht="39" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7"/>
       <c r="B48" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C48" s="9" t="n">
+      <c r="C48" s="9">
         <v>43010</v>
       </c>
-      <c r="D48" s="9" t="n">
+      <c r="D48" s="9">
         <v>43016</v>
       </c>
       <c r="E48" s="10"/>
-      <c r="F48" s="11" t="n">
+      <c r="F48" s="11">
         <v>0</v>
       </c>
       <c r="G48" s="10" t="s">
@@ -1918,19 +2115,19 @@
       <c r="H48" s="10"/>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="49" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A49" s="7"/>
       <c r="B49" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="13" t="n">
+      <c r="C49" s="13">
         <v>43010</v>
       </c>
-      <c r="D49" s="13" t="n">
+      <c r="D49" s="13">
         <v>43010</v>
       </c>
       <c r="E49" s="7"/>
-      <c r="F49" s="14" t="n">
+      <c r="F49" s="14">
         <v>0</v>
       </c>
       <c r="G49" s="7" t="s">
@@ -1943,19 +2140,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="50" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A50" s="7"/>
       <c r="B50" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="13" t="n">
+      <c r="C50" s="13">
         <v>43010</v>
       </c>
-      <c r="D50" s="13" t="n">
+      <c r="D50" s="13">
         <v>43010</v>
       </c>
       <c r="E50" s="7"/>
-      <c r="F50" s="14" t="n">
+      <c r="F50" s="14">
         <v>0</v>
       </c>
       <c r="G50" s="7" t="s">
@@ -1968,19 +2165,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="51" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A51" s="7"/>
       <c r="B51" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="13" t="n">
+      <c r="C51" s="13">
         <v>43012</v>
       </c>
-      <c r="D51" s="13" t="n">
+      <c r="D51" s="13">
         <v>43014</v>
       </c>
       <c r="E51" s="7"/>
-      <c r="F51" s="14" t="n">
+      <c r="F51" s="14">
         <v>0</v>
       </c>
       <c r="G51" s="7" t="s">
@@ -1993,19 +2190,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="52" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A52" s="7"/>
       <c r="B52" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C52" s="13" t="n">
+      <c r="C52" s="13">
         <v>43016</v>
       </c>
-      <c r="D52" s="13" t="n">
+      <c r="D52" s="13">
         <v>43016</v>
       </c>
       <c r="E52" s="7"/>
-      <c r="F52" s="14" t="n">
+      <c r="F52" s="14">
         <v>0</v>
       </c>
       <c r="G52" s="7" t="s">
@@ -2018,21 +2215,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="53" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A53" s="7"/>
       <c r="B53" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C53" s="13" t="n">
+      <c r="C53" s="13">
         <v>43016</v>
       </c>
-      <c r="D53" s="13" t="n">
+      <c r="D53" s="13">
         <v>43016</v>
       </c>
       <c r="E53" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F53" s="14" t="n">
+      <c r="F53" s="14">
         <v>0</v>
       </c>
       <c r="G53" s="7" t="s">
@@ -2043,19 +2240,19 @@
       </c>
       <c r="I53" s="7"/>
     </row>
-    <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="54" spans="1:9" ht="78" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7"/>
       <c r="B54" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="9" t="n">
+      <c r="C54" s="9">
         <v>43017</v>
       </c>
-      <c r="D54" s="9" t="n">
+      <c r="D54" s="9">
         <v>43023</v>
       </c>
       <c r="E54" s="10"/>
-      <c r="F54" s="11" t="n">
+      <c r="F54" s="11">
         <v>0</v>
       </c>
       <c r="G54" s="10" t="s">
@@ -2064,19 +2261,19 @@
       <c r="H54" s="10"/>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="55" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A55" s="7"/>
       <c r="B55" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C55" s="13" t="n">
+      <c r="C55" s="13">
         <v>43017</v>
       </c>
-      <c r="D55" s="13" t="n">
+      <c r="D55" s="13">
         <v>43017</v>
       </c>
       <c r="E55" s="7"/>
-      <c r="F55" s="14" t="n">
+      <c r="F55" s="14">
         <v>0</v>
       </c>
       <c r="G55" s="7" t="s">
@@ -2089,19 +2286,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="56" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A56" s="7"/>
       <c r="B56" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C56" s="13" t="n">
+      <c r="C56" s="13">
         <v>43017</v>
       </c>
-      <c r="D56" s="13" t="n">
+      <c r="D56" s="13">
         <v>43017</v>
       </c>
       <c r="E56" s="7"/>
-      <c r="F56" s="14" t="n">
+      <c r="F56" s="14">
         <v>0</v>
       </c>
       <c r="G56" s="7" t="s">
@@ -2114,19 +2311,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="57" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A57" s="7"/>
       <c r="B57" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="13" t="n">
+      <c r="C57" s="13">
         <v>43019</v>
       </c>
-      <c r="D57" s="13" t="n">
+      <c r="D57" s="13">
         <v>43021</v>
       </c>
       <c r="E57" s="7"/>
-      <c r="F57" s="14" t="n">
+      <c r="F57" s="14">
         <v>0</v>
       </c>
       <c r="G57" s="7" t="s">
@@ -2139,19 +2336,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="58" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A58" s="7"/>
       <c r="B58" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C58" s="13" t="n">
+      <c r="C58" s="13">
         <v>43023</v>
       </c>
-      <c r="D58" s="13" t="n">
+      <c r="D58" s="13">
         <v>43023</v>
       </c>
       <c r="E58" s="7"/>
-      <c r="F58" s="14" t="n">
+      <c r="F58" s="14">
         <v>0</v>
       </c>
       <c r="G58" s="7" t="s">
@@ -2164,21 +2361,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="59" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A59" s="7"/>
       <c r="B59" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C59" s="13" t="n">
+      <c r="C59" s="13">
         <v>43023</v>
       </c>
-      <c r="D59" s="13" t="n">
+      <c r="D59" s="13">
         <v>43023</v>
       </c>
       <c r="E59" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F59" s="14" t="n">
+      <c r="F59" s="14">
         <v>0</v>
       </c>
       <c r="G59" s="7" t="s">
@@ -2189,19 +2386,19 @@
       </c>
       <c r="I59" s="7"/>
     </row>
-    <row r="60" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:9" ht="52" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="4" t="n">
+      <c r="C60" s="4">
         <v>43024</v>
       </c>
-      <c r="D60" s="4" t="n">
+      <c r="D60" s="4">
         <v>43037</v>
       </c>
       <c r="E60" s="2"/>
-      <c r="F60" s="5" t="n">
+      <c r="F60" s="5">
         <v>0</v>
       </c>
       <c r="G60" s="2" t="s">
@@ -2210,19 +2407,19 @@
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="61" spans="1:9" ht="130" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7"/>
       <c r="B61" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C61" s="9" t="n">
+      <c r="C61" s="9">
         <v>43024</v>
       </c>
-      <c r="D61" s="9" t="n">
+      <c r="D61" s="9">
         <v>43030</v>
       </c>
       <c r="E61" s="10"/>
-      <c r="F61" s="11" t="n">
+      <c r="F61" s="11">
         <v>0</v>
       </c>
       <c r="G61" s="10" t="s">
@@ -2231,19 +2428,19 @@
       <c r="H61" s="10"/>
       <c r="I61" s="10"/>
     </row>
-    <row r="62" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="62" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A62" s="7"/>
       <c r="B62" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C62" s="13" t="n">
+      <c r="C62" s="13">
         <v>43024</v>
       </c>
-      <c r="D62" s="13" t="n">
+      <c r="D62" s="13">
         <v>43024</v>
       </c>
       <c r="E62" s="7"/>
-      <c r="F62" s="14" t="n">
+      <c r="F62" s="14">
         <v>0</v>
       </c>
       <c r="G62" s="7" t="s">
@@ -2256,19 +2453,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="63" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A63" s="7"/>
       <c r="B63" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C63" s="13" t="n">
+      <c r="C63" s="13">
         <v>43024</v>
       </c>
-      <c r="D63" s="13" t="n">
+      <c r="D63" s="13">
         <v>43024</v>
       </c>
       <c r="E63" s="7"/>
-      <c r="F63" s="14" t="n">
+      <c r="F63" s="14">
         <v>0</v>
       </c>
       <c r="G63" s="7" t="s">
@@ -2281,19 +2478,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="64" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A64" s="7"/>
       <c r="B64" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C64" s="13" t="n">
+      <c r="C64" s="13">
         <v>43026</v>
       </c>
-      <c r="D64" s="13" t="n">
+      <c r="D64" s="13">
         <v>43028</v>
       </c>
       <c r="E64" s="7"/>
-      <c r="F64" s="14" t="n">
+      <c r="F64" s="14">
         <v>0</v>
       </c>
       <c r="G64" s="7" t="s">
@@ -2306,19 +2503,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="65" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A65" s="7"/>
       <c r="B65" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C65" s="13" t="n">
+      <c r="C65" s="13">
         <v>43030</v>
       </c>
-      <c r="D65" s="13" t="n">
+      <c r="D65" s="13">
         <v>43030</v>
       </c>
       <c r="E65" s="7"/>
-      <c r="F65" s="14" t="n">
+      <c r="F65" s="14">
         <v>0</v>
       </c>
       <c r="G65" s="7" t="s">
@@ -2331,21 +2528,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="66" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A66" s="7"/>
       <c r="B66" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C66" s="13" t="n">
+      <c r="C66" s="13">
         <v>43030</v>
       </c>
-      <c r="D66" s="13" t="n">
+      <c r="D66" s="13">
         <v>43030</v>
       </c>
       <c r="E66" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F66" s="14" t="n">
+      <c r="F66" s="14">
         <v>0</v>
       </c>
       <c r="G66" s="7" t="s">
@@ -2356,19 +2553,19 @@
       </c>
       <c r="I66" s="7"/>
     </row>
-    <row r="67" s="16" customFormat="true" ht="39.6" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="67" spans="1:9" s="16" customFormat="1" ht="143" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A67" s="15"/>
       <c r="B67" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="9" t="n">
+      <c r="C67" s="9">
         <v>43031</v>
       </c>
-      <c r="D67" s="9" t="n">
+      <c r="D67" s="9">
         <v>43037</v>
       </c>
       <c r="E67" s="10"/>
-      <c r="F67" s="11" t="n">
+      <c r="F67" s="11">
         <v>0</v>
       </c>
       <c r="G67" s="10" t="s">
@@ -2377,19 +2574,19 @@
       <c r="H67" s="10"/>
       <c r="I67" s="10"/>
     </row>
-    <row r="68" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="68" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A68" s="7"/>
       <c r="B68" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C68" s="13" t="n">
+      <c r="C68" s="13">
         <v>43031</v>
       </c>
-      <c r="D68" s="13" t="n">
+      <c r="D68" s="13">
         <v>43031</v>
       </c>
       <c r="E68" s="7"/>
-      <c r="F68" s="14" t="n">
+      <c r="F68" s="14">
         <v>0</v>
       </c>
       <c r="G68" s="7" t="s">
@@ -2402,19 +2599,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="69" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A69" s="7"/>
       <c r="B69" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C69" s="13" t="n">
+      <c r="C69" s="13">
         <v>43031</v>
       </c>
-      <c r="D69" s="13" t="n">
+      <c r="D69" s="13">
         <v>43031</v>
       </c>
       <c r="E69" s="7"/>
-      <c r="F69" s="14" t="n">
+      <c r="F69" s="14">
         <v>0</v>
       </c>
       <c r="G69" s="7" t="s">
@@ -2427,19 +2624,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="70" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A70" s="7"/>
       <c r="B70" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C70" s="13" t="n">
+      <c r="C70" s="13">
         <v>43033</v>
       </c>
-      <c r="D70" s="13" t="n">
+      <c r="D70" s="13">
         <v>43035</v>
       </c>
       <c r="E70" s="7"/>
-      <c r="F70" s="14" t="n">
+      <c r="F70" s="14">
         <v>0</v>
       </c>
       <c r="G70" s="7" t="s">
@@ -2452,19 +2649,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="71" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A71" s="7"/>
       <c r="B71" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C71" s="13" t="n">
+      <c r="C71" s="13">
         <v>43037</v>
       </c>
-      <c r="D71" s="13" t="n">
+      <c r="D71" s="13">
         <v>43037</v>
       </c>
       <c r="E71" s="7"/>
-      <c r="F71" s="14" t="n">
+      <c r="F71" s="14">
         <v>0</v>
       </c>
       <c r="G71" s="7" t="s">
@@ -2477,21 +2674,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="72" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A72" s="7"/>
       <c r="B72" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C72" s="13" t="n">
+      <c r="C72" s="13">
         <v>43037</v>
       </c>
-      <c r="D72" s="13" t="n">
+      <c r="D72" s="13">
         <v>43037</v>
       </c>
       <c r="E72" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="F72" s="14" t="n">
+      <c r="F72" s="14">
         <v>0</v>
       </c>
       <c r="G72" s="7" t="s">
@@ -2502,19 +2699,19 @@
       </c>
       <c r="I72" s="7"/>
     </row>
-    <row r="73" customFormat="false" ht="26.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" spans="1:9" ht="52" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A73" s="2"/>
       <c r="B73" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C73" s="4" t="n">
+      <c r="C73" s="4">
         <v>43038</v>
       </c>
-      <c r="D73" s="4" t="n">
+      <c r="D73" s="4">
         <v>43052</v>
       </c>
       <c r="E73" s="2"/>
-      <c r="F73" s="5" t="n">
+      <c r="F73" s="5">
         <v>0</v>
       </c>
       <c r="G73" s="2" t="s">
@@ -2523,19 +2720,19 @@
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="74" spans="1:9" s="16" customFormat="1" ht="52" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15"/>
       <c r="B74" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C74" s="9" t="n">
+      <c r="C74" s="9">
         <v>43038</v>
       </c>
-      <c r="D74" s="9" t="n">
+      <c r="D74" s="9">
         <v>43042</v>
       </c>
       <c r="E74" s="10"/>
-      <c r="F74" s="11" t="n">
+      <c r="F74" s="11">
         <v>0</v>
       </c>
       <c r="G74" s="10" t="s">
@@ -2544,19 +2741,19 @@
       <c r="H74" s="10"/>
       <c r="I74" s="10"/>
     </row>
-    <row r="75" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="75" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A75" s="7"/>
       <c r="B75" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C75" s="9" t="n">
+      <c r="C75" s="9">
         <v>43038</v>
       </c>
-      <c r="D75" s="9" t="n">
+      <c r="D75" s="9">
         <v>43038</v>
       </c>
       <c r="E75" s="10"/>
-      <c r="F75" s="11" t="n">
+      <c r="F75" s="11">
         <v>0</v>
       </c>
       <c r="G75" s="10" t="s">
@@ -2569,19 +2766,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="76" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A76" s="7"/>
       <c r="B76" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C76" s="9" t="n">
+      <c r="C76" s="9">
         <v>43038</v>
       </c>
-      <c r="D76" s="9" t="n">
+      <c r="D76" s="9">
         <v>43038</v>
       </c>
       <c r="E76" s="10"/>
-      <c r="F76" s="11" t="n">
+      <c r="F76" s="11">
         <v>0</v>
       </c>
       <c r="G76" s="10" t="s">
@@ -2594,19 +2791,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="77" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A77" s="7"/>
       <c r="B77" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C77" s="9" t="n">
+      <c r="C77" s="9">
         <v>43040</v>
       </c>
-      <c r="D77" s="9" t="n">
+      <c r="D77" s="9">
         <v>43040</v>
       </c>
       <c r="E77" s="10"/>
-      <c r="F77" s="11" t="n">
+      <c r="F77" s="11">
         <v>0</v>
       </c>
       <c r="G77" s="10" t="s">
@@ -2619,19 +2816,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="78" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A78" s="7"/>
       <c r="B78" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C78" s="9" t="n">
+      <c r="C78" s="9">
         <v>43042</v>
       </c>
-      <c r="D78" s="9" t="n">
+      <c r="D78" s="9">
         <v>43042</v>
       </c>
       <c r="E78" s="10"/>
-      <c r="F78" s="11" t="n">
+      <c r="F78" s="11">
         <v>0</v>
       </c>
       <c r="G78" s="10" t="s">
@@ -2644,21 +2841,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="79" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A79" s="7"/>
       <c r="B79" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C79" s="9" t="n">
+      <c r="C79" s="9">
         <v>43042</v>
       </c>
-      <c r="D79" s="9" t="n">
+      <c r="D79" s="9">
         <v>43042</v>
       </c>
       <c r="E79" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F79" s="11" t="n">
+      <c r="F79" s="11">
         <v>0</v>
       </c>
       <c r="G79" s="10" t="s">
@@ -2669,19 +2866,19 @@
       </c>
       <c r="I79" s="10"/>
     </row>
-    <row r="80" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="80" spans="1:9" s="16" customFormat="1" ht="26" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A80" s="15"/>
       <c r="B80" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="9" t="n">
+      <c r="C80" s="9">
         <v>43044</v>
       </c>
-      <c r="D80" s="9" t="n">
+      <c r="D80" s="9">
         <v>43047</v>
       </c>
       <c r="E80" s="10"/>
-      <c r="F80" s="11" t="n">
+      <c r="F80" s="11">
         <v>0</v>
       </c>
       <c r="G80" s="10" t="s">
@@ -2690,19 +2887,19 @@
       <c r="H80" s="10"/>
       <c r="I80" s="10"/>
     </row>
-    <row r="81" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="81" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A81" s="7"/>
       <c r="B81" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C81" s="9" t="n">
+      <c r="C81" s="9">
         <v>43044</v>
       </c>
-      <c r="D81" s="9" t="n">
+      <c r="D81" s="9">
         <v>43044</v>
       </c>
       <c r="E81" s="10"/>
-      <c r="F81" s="11" t="n">
+      <c r="F81" s="11">
         <v>0</v>
       </c>
       <c r="G81" s="10" t="s">
@@ -2715,19 +2912,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="82" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A82" s="7"/>
       <c r="B82" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C82" s="9" t="n">
+      <c r="C82" s="9">
         <v>43044</v>
       </c>
-      <c r="D82" s="9" t="n">
+      <c r="D82" s="9">
         <v>43044</v>
       </c>
       <c r="E82" s="10"/>
-      <c r="F82" s="11" t="n">
+      <c r="F82" s="11">
         <v>0</v>
       </c>
       <c r="G82" s="10" t="s">
@@ -2740,19 +2937,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="83" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A83" s="7"/>
       <c r="B83" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C83" s="9" t="n">
+      <c r="C83" s="9">
         <v>43045</v>
       </c>
-      <c r="D83" s="9" t="n">
+      <c r="D83" s="9">
         <v>43045</v>
       </c>
       <c r="E83" s="10"/>
-      <c r="F83" s="11" t="n">
+      <c r="F83" s="11">
         <v>0</v>
       </c>
       <c r="G83" s="10" t="s">
@@ -2765,19 +2962,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="84" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A84" s="7"/>
       <c r="B84" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C84" s="9" t="n">
+      <c r="C84" s="9">
         <v>43047</v>
       </c>
-      <c r="D84" s="9" t="n">
+      <c r="D84" s="9">
         <v>43047</v>
       </c>
       <c r="E84" s="10"/>
-      <c r="F84" s="11" t="n">
+      <c r="F84" s="11">
         <v>0</v>
       </c>
       <c r="G84" s="10" t="s">
@@ -2790,21 +2987,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="85" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A85" s="7"/>
       <c r="B85" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C85" s="9" t="n">
+      <c r="C85" s="9">
         <v>43047</v>
       </c>
-      <c r="D85" s="9" t="n">
+      <c r="D85" s="9">
         <v>43047</v>
       </c>
       <c r="E85" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F85" s="11" t="n">
+      <c r="F85" s="11">
         <v>0</v>
       </c>
       <c r="G85" s="10" t="s">
@@ -2815,19 +3012,19 @@
       </c>
       <c r="I85" s="10"/>
     </row>
-    <row r="86" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="86" spans="1:9" s="16" customFormat="1" ht="39" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A86" s="15"/>
       <c r="B86" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C86" s="9" t="n">
+      <c r="C86" s="9">
         <v>43049</v>
       </c>
-      <c r="D86" s="9" t="n">
+      <c r="D86" s="9">
         <v>43052</v>
       </c>
       <c r="E86" s="10"/>
-      <c r="F86" s="11" t="n">
+      <c r="F86" s="11">
         <v>0</v>
       </c>
       <c r="G86" s="10" t="s">
@@ -2836,19 +3033,19 @@
       <c r="H86" s="10"/>
       <c r="I86" s="10"/>
     </row>
-    <row r="87" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="87" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A87" s="7"/>
       <c r="B87" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C87" s="13" t="n">
+      <c r="C87" s="13">
         <v>43049</v>
       </c>
-      <c r="D87" s="13" t="n">
+      <c r="D87" s="13">
         <v>43049</v>
       </c>
       <c r="E87" s="7"/>
-      <c r="F87" s="14" t="n">
+      <c r="F87" s="14">
         <v>0</v>
       </c>
       <c r="G87" s="7" t="s">
@@ -2861,19 +3058,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="88" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A88" s="7"/>
       <c r="B88" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C88" s="13" t="n">
+      <c r="C88" s="13">
         <v>43049</v>
       </c>
-      <c r="D88" s="13" t="n">
+      <c r="D88" s="13">
         <v>43049</v>
       </c>
       <c r="E88" s="7"/>
-      <c r="F88" s="14" t="n">
+      <c r="F88" s="14">
         <v>0</v>
       </c>
       <c r="G88" s="7" t="s">
@@ -2886,19 +3083,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="89" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A89" s="7"/>
       <c r="B89" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C89" s="13" t="n">
+      <c r="C89" s="13">
         <v>43051</v>
       </c>
-      <c r="D89" s="13" t="n">
+      <c r="D89" s="13">
         <v>43051</v>
       </c>
       <c r="E89" s="7"/>
-      <c r="F89" s="14" t="n">
+      <c r="F89" s="14">
         <v>0</v>
       </c>
       <c r="G89" s="7" t="s">
@@ -2911,19 +3108,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="90" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A90" s="7"/>
       <c r="B90" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C90" s="13" t="n">
+      <c r="C90" s="13">
         <v>43052</v>
       </c>
-      <c r="D90" s="13" t="n">
+      <c r="D90" s="13">
         <v>43052</v>
       </c>
       <c r="E90" s="7"/>
-      <c r="F90" s="14" t="n">
+      <c r="F90" s="14">
         <v>0</v>
       </c>
       <c r="G90" s="7" t="s">
@@ -2936,21 +3133,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="91" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A91" s="7"/>
       <c r="B91" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C91" s="13" t="n">
+      <c r="C91" s="13">
         <v>43052</v>
       </c>
-      <c r="D91" s="13" t="n">
+      <c r="D91" s="13">
         <v>43052</v>
       </c>
       <c r="E91" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F91" s="14" t="n">
+      <c r="F91" s="14">
         <v>0</v>
       </c>
       <c r="G91" s="7" t="s">
@@ -2961,19 +3158,19 @@
       </c>
       <c r="I91" s="7"/>
     </row>
-    <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:9" ht="39" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A92" s="2"/>
       <c r="B92" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C92" s="4" t="n">
+      <c r="C92" s="4">
         <v>43054</v>
       </c>
-      <c r="D92" s="4" t="n">
-        <v>42764</v>
+      <c r="D92" s="4">
+        <v>43068</v>
       </c>
       <c r="E92" s="2"/>
-      <c r="F92" s="5" t="n">
+      <c r="F92" s="5">
         <v>0</v>
       </c>
       <c r="G92" s="2" t="s">
@@ -2982,19 +3179,19 @@
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="93" spans="1:9" s="16" customFormat="1" ht="78" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A93" s="15"/>
       <c r="B93" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="C93" s="9" t="n">
+      <c r="C93" s="9">
         <v>43054</v>
       </c>
-      <c r="D93" s="9" t="n">
+      <c r="D93" s="9">
         <v>43058</v>
       </c>
       <c r="E93" s="10"/>
-      <c r="F93" s="11" t="n">
+      <c r="F93" s="11">
         <v>0</v>
       </c>
       <c r="G93" s="10" t="s">
@@ -3003,19 +3200,19 @@
       <c r="H93" s="10"/>
       <c r="I93" s="10"/>
     </row>
-    <row r="94" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="94" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A94" s="15"/>
       <c r="B94" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C94" s="9" t="n">
+      <c r="C94" s="9">
         <v>43054</v>
       </c>
-      <c r="D94" s="9" t="n">
+      <c r="D94" s="9">
         <v>43054</v>
       </c>
       <c r="E94" s="10"/>
-      <c r="F94" s="11" t="n">
+      <c r="F94" s="11">
         <v>0</v>
       </c>
       <c r="G94" s="10" t="s">
@@ -3028,19 +3225,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="95" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A95" s="15"/>
       <c r="B95" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C95" s="9" t="n">
+      <c r="C95" s="9">
         <v>43054</v>
       </c>
-      <c r="D95" s="9" t="n">
+      <c r="D95" s="9">
         <v>43054</v>
       </c>
       <c r="E95" s="10"/>
-      <c r="F95" s="11" t="n">
+      <c r="F95" s="11">
         <v>0</v>
       </c>
       <c r="G95" s="10" t="s">
@@ -3053,19 +3250,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="96" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A96" s="15"/>
       <c r="B96" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C96" s="9" t="n">
+      <c r="C96" s="9">
         <v>43056</v>
       </c>
-      <c r="D96" s="9" t="n">
+      <c r="D96" s="9">
         <v>43056</v>
       </c>
       <c r="E96" s="10"/>
-      <c r="F96" s="11" t="n">
+      <c r="F96" s="11">
         <v>0</v>
       </c>
       <c r="G96" s="10" t="s">
@@ -3078,19 +3275,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="97" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A97" s="15"/>
       <c r="B97" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C97" s="9" t="n">
+      <c r="C97" s="9">
         <v>43058</v>
       </c>
-      <c r="D97" s="9" t="n">
+      <c r="D97" s="9">
         <v>43058</v>
       </c>
       <c r="E97" s="10"/>
-      <c r="F97" s="11" t="n">
+      <c r="F97" s="11">
         <v>0</v>
       </c>
       <c r="G97" s="10" t="s">
@@ -3103,21 +3300,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="98" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A98" s="15"/>
       <c r="B98" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C98" s="9" t="n">
+      <c r="C98" s="9">
         <v>43058</v>
       </c>
-      <c r="D98" s="9" t="n">
+      <c r="D98" s="9">
         <v>43058</v>
       </c>
       <c r="E98" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F98" s="11" t="n">
+      <c r="F98" s="11">
         <v>0</v>
       </c>
       <c r="G98" s="10" t="s">
@@ -3128,19 +3325,19 @@
       </c>
       <c r="I98" s="10"/>
     </row>
-    <row r="99" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="99" spans="1:9" ht="78" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A99" s="15"/>
       <c r="B99" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="C99" s="9" t="n">
+      <c r="C99" s="9">
         <v>43059</v>
       </c>
-      <c r="D99" s="9" t="n">
+      <c r="D99" s="9">
         <v>43063</v>
       </c>
       <c r="E99" s="10"/>
-      <c r="F99" s="11" t="n">
+      <c r="F99" s="11">
         <v>0</v>
       </c>
       <c r="G99" s="10" t="s">
@@ -3149,19 +3346,19 @@
       <c r="H99" s="10"/>
       <c r="I99" s="10"/>
     </row>
-    <row r="100" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="100" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A100" s="15"/>
       <c r="B100" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C100" s="9" t="n">
+      <c r="C100" s="9">
         <v>43059</v>
       </c>
-      <c r="D100" s="9" t="n">
+      <c r="D100" s="9">
         <v>43059</v>
       </c>
       <c r="E100" s="10"/>
-      <c r="F100" s="11" t="n">
+      <c r="F100" s="11">
         <v>0</v>
       </c>
       <c r="G100" s="10" t="s">
@@ -3174,19 +3371,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="101" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A101" s="15"/>
       <c r="B101" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C101" s="9" t="n">
+      <c r="C101" s="9">
         <v>43059</v>
       </c>
-      <c r="D101" s="9" t="n">
+      <c r="D101" s="9">
         <v>43059</v>
       </c>
       <c r="E101" s="10"/>
-      <c r="F101" s="11" t="n">
+      <c r="F101" s="11">
         <v>0</v>
       </c>
       <c r="G101" s="10" t="s">
@@ -3199,19 +3396,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="102" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A102" s="15"/>
       <c r="B102" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C102" s="9" t="n">
+      <c r="C102" s="9">
         <v>43061</v>
       </c>
-      <c r="D102" s="9" t="n">
+      <c r="D102" s="9">
         <v>43061</v>
       </c>
       <c r="E102" s="10"/>
-      <c r="F102" s="11" t="n">
+      <c r="F102" s="11">
         <v>0</v>
       </c>
       <c r="G102" s="10" t="s">
@@ -3224,19 +3421,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="103" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A103" s="15"/>
       <c r="B103" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C103" s="9" t="n">
+      <c r="C103" s="9">
         <v>43063</v>
       </c>
-      <c r="D103" s="9" t="n">
+      <c r="D103" s="9">
         <v>43063</v>
       </c>
       <c r="E103" s="10"/>
-      <c r="F103" s="11" t="n">
+      <c r="F103" s="11">
         <v>0</v>
       </c>
       <c r="G103" s="10" t="s">
@@ -3249,21 +3446,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="104" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A104" s="15"/>
       <c r="B104" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C104" s="9" t="n">
+      <c r="C104" s="9">
         <v>43063</v>
       </c>
-      <c r="D104" s="9" t="n">
+      <c r="D104" s="9">
         <v>43063</v>
       </c>
       <c r="E104" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="F104" s="11" t="n">
+      <c r="F104" s="11">
         <v>0</v>
       </c>
       <c r="G104" s="10" t="s">
@@ -3274,19 +3471,19 @@
       </c>
       <c r="I104" s="10"/>
     </row>
-    <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="1" collapsed="true">
+    <row r="105" spans="1:9" ht="78" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A105" s="15"/>
       <c r="B105" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="C105" s="9" t="n">
+      <c r="C105" s="9">
         <v>43065</v>
       </c>
-      <c r="D105" s="9" t="n">
+      <c r="D105" s="9">
         <v>43068</v>
       </c>
       <c r="E105" s="10"/>
-      <c r="F105" s="11" t="n">
+      <c r="F105" s="11">
         <v>0</v>
       </c>
       <c r="G105" s="10" t="s">
@@ -3295,19 +3492,19 @@
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
     </row>
-    <row r="106" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="106" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A106" s="7"/>
       <c r="B106" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C106" s="13" t="n">
+      <c r="C106" s="13">
         <v>43065</v>
       </c>
-      <c r="D106" s="13" t="n">
+      <c r="D106" s="13">
         <v>43065</v>
       </c>
       <c r="E106" s="7"/>
-      <c r="F106" s="14" t="n">
+      <c r="F106" s="14">
         <v>0</v>
       </c>
       <c r="G106" s="7" t="s">
@@ -3320,19 +3517,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="107" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C107" s="13" t="n">
+      <c r="C107" s="13">
         <v>43065</v>
       </c>
-      <c r="D107" s="13" t="n">
+      <c r="D107" s="13">
         <v>43065</v>
       </c>
       <c r="E107" s="7"/>
-      <c r="F107" s="14" t="n">
+      <c r="F107" s="14">
         <v>0</v>
       </c>
       <c r="G107" s="7" t="s">
@@ -3345,19 +3542,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="108" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A108" s="7"/>
       <c r="B108" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C108" s="13" t="n">
+      <c r="C108" s="13">
         <v>43066</v>
       </c>
-      <c r="D108" s="13" t="n">
+      <c r="D108" s="13">
         <v>43066</v>
       </c>
       <c r="E108" s="7"/>
-      <c r="F108" s="14" t="n">
+      <c r="F108" s="14">
         <v>0</v>
       </c>
       <c r="G108" s="7" t="s">
@@ -3370,19 +3567,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="109" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A109" s="7"/>
       <c r="B109" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C109" s="13" t="n">
+      <c r="C109" s="13">
         <v>43068</v>
       </c>
-      <c r="D109" s="13" t="n">
+      <c r="D109" s="13">
         <v>43068</v>
       </c>
       <c r="E109" s="7"/>
-      <c r="F109" s="14" t="n">
+      <c r="F109" s="14">
         <v>0</v>
       </c>
       <c r="G109" s="7" t="s">
@@ -3395,21 +3592,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="110" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A110" s="7"/>
       <c r="B110" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C110" s="13" t="n">
+      <c r="C110" s="13">
         <v>43068</v>
       </c>
-      <c r="D110" s="13" t="n">
+      <c r="D110" s="13">
         <v>43068</v>
       </c>
       <c r="E110" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F110" s="14" t="n">
+      <c r="F110" s="14">
         <v>0</v>
       </c>
       <c r="G110" s="7" t="s">
@@ -3420,19 +3617,19 @@
       </c>
       <c r="I110" s="7"/>
     </row>
-    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="111" spans="1:9" ht="39" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A111" s="2"/>
       <c r="B111" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C111" s="4" t="n">
+      <c r="C111" s="4">
         <v>43070</v>
       </c>
-      <c r="D111" s="4" t="n">
+      <c r="D111" s="4">
         <v>43073</v>
       </c>
       <c r="E111" s="2"/>
-      <c r="F111" s="5" t="n">
+      <c r="F111" s="5">
         <v>0</v>
       </c>
       <c r="G111" s="2" t="s">
@@ -3441,19 +3638,19 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="112" spans="1:9" s="16" customFormat="1" ht="26" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A112" s="15"/>
       <c r="B112" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C112" s="9" t="n">
+      <c r="C112" s="9">
         <v>43070</v>
       </c>
-      <c r="D112" s="9" t="n">
+      <c r="D112" s="9">
         <v>43073</v>
       </c>
       <c r="E112" s="10"/>
-      <c r="F112" s="11" t="n">
+      <c r="F112" s="11">
         <v>0</v>
       </c>
       <c r="G112" s="10" t="s">
@@ -3462,19 +3659,19 @@
       <c r="H112" s="10"/>
       <c r="I112" s="10"/>
     </row>
-    <row r="113" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="113" spans="1:9" ht="65" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A113" s="7"/>
       <c r="B113" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C113" s="13" t="n">
+      <c r="C113" s="13">
         <v>43070</v>
       </c>
-      <c r="D113" s="13" t="n">
+      <c r="D113" s="13">
         <v>43070</v>
       </c>
       <c r="E113" s="7"/>
-      <c r="F113" s="14" t="n">
+      <c r="F113" s="14">
         <v>0</v>
       </c>
       <c r="G113" s="7" t="s">
@@ -3487,19 +3684,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="114" spans="1:9" ht="52" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A114" s="7"/>
       <c r="B114" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C114" s="13" t="n">
+      <c r="C114" s="13">
         <v>43070</v>
       </c>
-      <c r="D114" s="13" t="n">
+      <c r="D114" s="13">
         <v>43070</v>
       </c>
       <c r="E114" s="7"/>
-      <c r="F114" s="14" t="n">
+      <c r="F114" s="14">
         <v>0</v>
       </c>
       <c r="G114" s="7" t="s">
@@ -3512,19 +3709,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="115" spans="1:9" ht="130" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A115" s="7"/>
       <c r="B115" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C115" s="13" t="n">
+      <c r="C115" s="13">
         <v>43072</v>
       </c>
-      <c r="D115" s="13" t="n">
+      <c r="D115" s="13">
         <v>43072</v>
       </c>
       <c r="E115" s="7"/>
-      <c r="F115" s="14" t="n">
+      <c r="F115" s="14">
         <v>0</v>
       </c>
       <c r="G115" s="7" t="s">
@@ -3537,19 +3734,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="116" spans="1:9" ht="91" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A116" s="7"/>
       <c r="B116" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C116" s="13" t="n">
+      <c r="C116" s="13">
         <v>43073</v>
       </c>
-      <c r="D116" s="13" t="n">
+      <c r="D116" s="13">
         <v>43073</v>
       </c>
       <c r="E116" s="7"/>
-      <c r="F116" s="14" t="n">
+      <c r="F116" s="14">
         <v>0</v>
       </c>
       <c r="G116" s="7" t="s">
@@ -3562,21 +3759,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" customFormat="false" ht="14.4" hidden="true" customHeight="false" outlineLevel="2" collapsed="false">
+    <row r="117" spans="1:9" ht="117" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A117" s="7"/>
       <c r="B117" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C117" s="13" t="n">
+      <c r="C117" s="13">
         <v>43073</v>
       </c>
-      <c r="D117" s="13" t="n">
+      <c r="D117" s="13">
         <v>43073</v>
       </c>
       <c r="E117" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F117" s="14" t="n">
+      <c r="F117" s="14">
         <v>0</v>
       </c>
       <c r="G117" s="7" t="s">
@@ -3587,19 +3784,19 @@
       </c>
       <c r="I117" s="7"/>
     </row>
-    <row r="118" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" spans="1:9" ht="26" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A118" s="2"/>
       <c r="B118" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C118" s="4" t="n">
+      <c r="C118" s="4">
         <v>43074</v>
       </c>
-      <c r="D118" s="4" t="n">
+      <c r="D118" s="4">
         <v>43075</v>
       </c>
       <c r="E118" s="2"/>
-      <c r="F118" s="5" t="n">
+      <c r="F118" s="5">
         <v>0</v>
       </c>
       <c r="G118" s="2" t="s">
@@ -3608,19 +3805,19 @@
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" s="16" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" spans="1:9" s="16" customFormat="1" ht="52" x14ac:dyDescent="0.2">
       <c r="A119" s="15"/>
       <c r="B119" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="C119" s="9" t="n">
+      <c r="C119" s="9">
         <v>43074</v>
       </c>
-      <c r="D119" s="9" t="n">
+      <c r="D119" s="9">
         <v>43075</v>
       </c>
       <c r="E119" s="10"/>
-      <c r="F119" s="11" t="n">
+      <c r="F119" s="11">
         <v>0</v>
       </c>
       <c r="G119" s="10" t="s">
@@ -3632,42 +3829,20 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.0688259109312"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="60.5222672064777"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.89068825910931"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>